<commit_message>
Adding new weapons and armours
</commit_message>
<xml_diff>
--- a/IceWind_Dale/equipment.xlsx
+++ b/IceWind_Dale/equipment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\Github\rpg-data\IceWind_Dale\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Zbroja" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Broń!$B$1:$K$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Broń!$C$1:$L$32</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="194">
   <si>
     <t>Nazwa broni</t>
   </si>
@@ -198,9 +198,6 @@
     <t>miecz półtoraręczny</t>
   </si>
   <si>
-    <t>Miecz obóręczny</t>
-  </si>
-  <si>
     <t>1k10</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>FAR</t>
-  </si>
-  <si>
     <t>MYŚ</t>
   </si>
   <si>
@@ -475,6 +469,147 @@
   </si>
   <si>
     <t>Klasa pancerza: +1, nie chroni przed pociskami</t>
+  </si>
+  <si>
+    <t>Zbroja płytowa</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Miecz oburęczny</t>
+  </si>
+  <si>
+    <t>Krótki łuk +1</t>
+  </si>
+  <si>
+    <t>Miecz półtoraręczny +1</t>
+  </si>
+  <si>
+    <t>2k6+1</t>
+  </si>
+  <si>
+    <t>Miecz krótki +1</t>
+  </si>
+  <si>
+    <t>Zbroja płytowa +1</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>FER</t>
+  </si>
+  <si>
+    <t>Bransolety ochrony</t>
+  </si>
+  <si>
+    <t>ZMA</t>
+  </si>
+  <si>
+    <t>Chełm zaufanego obrońcy</t>
+  </si>
+  <si>
+    <t>klasa pancerza: +3, niewrażliwość na uśpienie i zmęczenie, chroni przed obrażeniami krytycznymi</t>
+  </si>
+  <si>
+    <t>Krasnolud</t>
+  </si>
+  <si>
+    <t>Elf</t>
+  </si>
+  <si>
+    <t>Półork</t>
+  </si>
+  <si>
+    <t>Półelf</t>
+  </si>
+  <si>
+    <t>Człowiek</t>
+  </si>
+  <si>
+    <t>Odporność na magię: +5%, 5% szans na rzucenie czaru Rozproszenie magii, po trafieniu</t>
+  </si>
+  <si>
+    <t>1k8+3</t>
+  </si>
+  <si>
+    <t>1k8+2</t>
+  </si>
+  <si>
+    <t>Pogromca wiary +2</t>
+  </si>
+  <si>
+    <t>Zabójca olbrzymów +1, +4 przeciw olbrzymom</t>
+  </si>
+  <si>
+    <t>+1, +4 przeciw olbrzymom</t>
+  </si>
+  <si>
+    <t>Włócznia z białego jesionu +3</t>
+  </si>
+  <si>
+    <t>5% szans na dodatkowe 1k6 obrażeń kłutych na kolców na grocie włóczni</t>
+  </si>
+  <si>
+    <t>+3</t>
+  </si>
+  <si>
+    <t>Oko świni +4</t>
+  </si>
+  <si>
+    <t>50% szans, że trafiony ork zostanie oślepiony</t>
+  </si>
+  <si>
+    <t>1k6+2, +4 przeciw orkom</t>
+  </si>
+  <si>
+    <t>+2, +4 przeciw orkom</t>
+  </si>
+  <si>
+    <t>Hiena cmentarna +3</t>
+  </si>
+  <si>
+    <t>1k6+4</t>
+  </si>
+  <si>
+    <t>Sejmitar szczęścia +2</t>
+  </si>
+  <si>
+    <t>szczęście (+1 do wszystkich rzutów), właściwości ładunków - szczęście (raz dziennie), zasięg: 5 metrów, czas trwania: 3 rundy, obszar działania: 1 istota</t>
+  </si>
+  <si>
+    <t>Ostoja +4</t>
+  </si>
+  <si>
+    <t>1k4+4</t>
+  </si>
+  <si>
+    <t>+4</t>
+  </si>
+  <si>
+    <t>Kwiatek +3</t>
+  </si>
+  <si>
+    <t>+5</t>
+  </si>
+  <si>
+    <t>Czarny łuk +3</t>
+  </si>
+  <si>
+    <t>Halabarda Fayra +3</t>
+  </si>
+  <si>
+    <t>1k10+3</t>
+  </si>
+  <si>
+    <t>Kij Erona +3</t>
+  </si>
+  <si>
+    <t>1k6+3</t>
+  </si>
+  <si>
+    <t>Piekielny młot +3</t>
   </si>
 </sst>
 </file>
@@ -874,82 +1009,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF32"/>
+  <dimension ref="A1:AG47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X47" sqref="X47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="3" width="10.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="4.88671875" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" customWidth="1"/>
-    <col min="15" max="15" width="8.21875" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-    <col min="17" max="17" width="9.88671875" customWidth="1"/>
-    <col min="18" max="18" width="4.88671875" customWidth="1"/>
-    <col min="19" max="19" width="4.77734375" customWidth="1"/>
-    <col min="20" max="20" width="9.44140625" customWidth="1"/>
-    <col min="21" max="21" width="9.5546875" customWidth="1"/>
-    <col min="22" max="22" width="14.77734375" customWidth="1"/>
-    <col min="23" max="23" width="5.44140625" customWidth="1"/>
-    <col min="24" max="24" width="5.5546875" customWidth="1"/>
-    <col min="25" max="25" width="6.109375" customWidth="1"/>
-    <col min="26" max="26" width="6.21875" customWidth="1"/>
-    <col min="27" max="27" width="6" customWidth="1"/>
-    <col min="28" max="28" width="5.109375" customWidth="1"/>
-    <col min="29" max="29" width="5.44140625" customWidth="1"/>
-    <col min="30" max="30" width="10.44140625" customWidth="1"/>
-    <col min="31" max="31" width="14.5546875" customWidth="1"/>
-    <col min="32" max="32" width="10" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="4.88671875" customWidth="1"/>
+    <col min="14" max="14" width="5.109375" customWidth="1"/>
+    <col min="15" max="15" width="5.88671875" customWidth="1"/>
+    <col min="16" max="16" width="8.21875" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" customWidth="1"/>
+    <col min="19" max="19" width="4.88671875" customWidth="1"/>
+    <col min="20" max="20" width="4.77734375" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" customWidth="1"/>
+    <col min="22" max="22" width="9.5546875" customWidth="1"/>
+    <col min="23" max="23" width="14.77734375" customWidth="1"/>
+    <col min="24" max="24" width="5.44140625" customWidth="1"/>
+    <col min="25" max="25" width="5.5546875" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" customWidth="1"/>
+    <col min="27" max="27" width="6.21875" customWidth="1"/>
+    <col min="28" max="28" width="6" customWidth="1"/>
+    <col min="29" max="29" width="5.109375" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.5546875" customWidth="1"/>
+    <col min="33" max="33" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="11"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
@@ -962,176 +1102,174 @@
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
       <c r="Y1" s="11"/>
-    </row>
-    <row r="2" spans="1:32" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4"/>
+      <c r="Z1" s="11"/>
+    </row>
+    <row r="2" spans="1:33" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="4"/>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="Q2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AD2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AF2" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>3</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="T3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="R3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>6</v>
       </c>
-      <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
-      <c r="W4" s="2"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="U4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>25</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>7</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>29</v>
@@ -1139,41 +1277,41 @@
       <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="2"/>
+      <c r="O5" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>28</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>4</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>29</v>
@@ -1184,10 +1322,10 @@
       <c r="O6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="U6" s="1" t="s">
@@ -1199,336 +1337,338 @@
       <c r="W6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>43</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>13</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>14</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3</v>
       </c>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>7</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>46</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>25</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>8</v>
       </c>
-      <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="O8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
-      <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="U8" s="2"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>48</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>14</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>5</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="O9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="T9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X9" s="2"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>7</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>52</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>13</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>53</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>12</v>
       </c>
-      <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="R10" s="2"/>
+      <c r="O10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
-      <c r="W10" s="2"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="U10" s="2"/>
+      <c r="X10" s="2"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>8</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>55</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>13</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>53</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>10</v>
       </c>
-      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="O11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X11" s="2"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" t="s">
         <v>57</v>
       </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12">
+      <c r="L12">
         <v>15</v>
       </c>
-      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="Q12" s="2"/>
+      <c r="O12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>5</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" t="s">
         <v>61</v>
       </c>
-      <c r="I13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13">
+      <c r="L13">
         <v>4</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="M13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="U13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="R13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>13</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>28</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>6</v>
       </c>
-      <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="T14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="R14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15">
-        <v>7</v>
-      </c>
-      <c r="H15" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K15">
+      <c r="L15">
         <v>15</v>
       </c>
-      <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="R15" s="2"/>
+      <c r="O15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
-      <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="U15" s="2"/>
+      <c r="X15" s="2"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" t="s">
         <v>70</v>
       </c>
-      <c r="G16">
+      <c r="L16">
         <v>4</v>
       </c>
-      <c r="H16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" t="s">
-        <v>71</v>
-      </c>
-      <c r="K16">
-        <v>4</v>
-      </c>
-      <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="Q16" s="2"/>
+      <c r="O16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
@@ -1537,514 +1677,1071 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z16" s="2"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17">
+      <c r="J17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17">
         <v>4</v>
       </c>
-      <c r="H17" t="s">
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="I17" t="s">
+      <c r="C18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" t="s">
         <v>49</v>
       </c>
-      <c r="J17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17">
-        <v>4</v>
-      </c>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
-        <v>77</v>
-      </c>
-      <c r="I18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18">
+      <c r="K18" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18">
         <v>15</v>
       </c>
-      <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="Q18" s="2"/>
+      <c r="O18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" t="s">
         <v>79</v>
       </c>
-      <c r="I19" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19">
+      <c r="L19">
         <v>1</v>
       </c>
-      <c r="L19" s="2"/>
-      <c r="O19" s="2"/>
+      <c r="M19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="U19" s="2"/>
+      <c r="R19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20">
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20">
         <v>2</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
         <v>79</v>
       </c>
-      <c r="I20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" t="s">
-        <v>80</v>
-      </c>
-      <c r="K20">
+      <c r="L20">
         <v>0</v>
       </c>
-      <c r="L20" s="2"/>
-      <c r="O20" s="2"/>
+      <c r="M20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="U20" s="2"/>
+      <c r="R20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z20" s="2"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
         <v>84</v>
       </c>
-      <c r="E21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21" t="s">
-        <v>85</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>13</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>0</v>
       </c>
-      <c r="L21" s="2"/>
-      <c r="O21" s="2"/>
+      <c r="M21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="U21" s="2"/>
+      <c r="R21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="X21" s="2"/>
+      <c r="W21" s="2"/>
       <c r="Y21" s="2"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22">
+      <c r="D22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22">
         <v>10</v>
       </c>
-      <c r="H22" t="s">
-        <v>91</v>
-      </c>
       <c r="I22" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" t="s">
         <v>49</v>
       </c>
-      <c r="J22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K22">
+      <c r="K22" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22">
         <v>14</v>
       </c>
-      <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="Q22" s="2"/>
+      <c r="P22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="T22" s="2"/>
+      <c r="S22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="X22" s="2"/>
+      <c r="W22" s="2"/>
       <c r="Y22" s="2"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z22" s="2"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23">
-        <v>5</v>
-      </c>
-      <c r="H23" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>49</v>
       </c>
-      <c r="J23" t="s">
-        <v>62</v>
-      </c>
-      <c r="K23">
+      <c r="K23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23">
         <v>7</v>
       </c>
-      <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="Q23" s="2"/>
+      <c r="P23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="T23" s="2"/>
+      <c r="S23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="X23" s="2"/>
+      <c r="W23" s="2"/>
       <c r="Y23" s="2"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z23" s="2"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="H24">
+        <v>7</v>
+      </c>
+      <c r="I24" t="s">
         <v>93</v>
       </c>
-      <c r="G24">
-        <v>7</v>
-      </c>
-      <c r="H24" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>49</v>
       </c>
-      <c r="J24" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24">
+      <c r="K24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24">
         <v>3</v>
       </c>
-      <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="Q24" s="2"/>
+      <c r="O24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="X24" s="2"/>
+      <c r="W24" s="2"/>
       <c r="Y24" s="2"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z24" s="2"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25">
+        <v>7</v>
+      </c>
+      <c r="I25" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G25">
-        <v>7</v>
-      </c>
-      <c r="H25" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25" t="s">
-        <v>49</v>
-      </c>
-      <c r="J25" t="s">
-        <v>96</v>
-      </c>
-      <c r="K25">
+      <c r="L25">
         <v>10</v>
       </c>
-      <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="Q25" s="2"/>
+      <c r="O25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="X25" s="2"/>
+      <c r="W25" s="2"/>
       <c r="Y25" s="2"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z25" s="2"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
         <v>97</v>
       </c>
-      <c r="G26">
-        <v>6</v>
-      </c>
-      <c r="H26" t="s">
-        <v>98</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>49</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>28</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>2</v>
       </c>
-      <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="T26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="R26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="X26" s="2"/>
+      <c r="W26" s="2"/>
       <c r="Y26" s="2"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z26" s="2"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
         <v>99</v>
       </c>
-      <c r="G27">
-        <v>6</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="J27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" t="s">
+        <v>79</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>100</v>
       </c>
-      <c r="I27" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" t="s">
-        <v>80</v>
-      </c>
-      <c r="K27">
+      <c r="C28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
+      </c>
+      <c r="L28">
         <v>0</v>
       </c>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" t="s">
-        <v>91</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="R28" s="2"/>
       <c r="S28" s="2"/>
-      <c r="Z28" s="2"/>
+      <c r="T28" s="2"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG28" s="2"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" t="s">
-        <v>110</v>
-      </c>
-      <c r="K29">
+      <c r="L29">
         <v>0</v>
       </c>
-      <c r="R29" s="2"/>
       <c r="S29" s="2"/>
-      <c r="Z29" s="1"/>
+      <c r="T29" s="2"/>
       <c r="AA29" s="1"/>
-      <c r="AB29" s="2"/>
+      <c r="AB29" s="1"/>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG29" s="2"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" t="s">
+        <v>99</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" t="s">
-        <v>100</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="D31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" t="s">
         <v>11</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>1</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
+        <v>78</v>
+      </c>
+      <c r="J31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" t="s">
         <v>79</v>
       </c>
-      <c r="I31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" t="s">
-        <v>80</v>
-      </c>
-      <c r="K31">
+      <c r="L31">
         <v>1</v>
       </c>
-      <c r="L31" s="2"/>
-      <c r="O31" s="2"/>
+      <c r="M31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
-      <c r="U31" s="2"/>
+      <c r="R31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="X31" s="2"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="D32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" t="s">
         <v>11</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>2</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
         <v>79</v>
       </c>
-      <c r="I32" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K32">
+      <c r="L32">
         <v>1</v>
       </c>
-      <c r="L32" s="2"/>
-      <c r="O32" s="2"/>
+      <c r="M32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="U32" s="2"/>
+      <c r="R32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" t="s">
+        <v>49</v>
+      </c>
+      <c r="K33" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34">
+        <v>7</v>
+      </c>
+      <c r="I34" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" t="s">
+        <v>53</v>
+      </c>
+      <c r="L34">
+        <v>9</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35">
+        <v>3</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+    </row>
+    <row r="36" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="I36" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36">
+        <v>5</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+    </row>
+    <row r="37" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>99</v>
+      </c>
+      <c r="J37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" t="s">
+        <v>79</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+    </row>
+    <row r="38" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>48</v>
+      </c>
+      <c r="J38" t="s">
+        <v>49</v>
+      </c>
+      <c r="K38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+    </row>
+    <row r="39" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>175</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39">
+        <v>3</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" t="s">
+        <v>65</v>
+      </c>
+      <c r="L40">
+        <v>5</v>
+      </c>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="X40" s="2"/>
+    </row>
+    <row r="41" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>181</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41" t="s">
+        <v>60</v>
+      </c>
+      <c r="J41" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41" t="s">
+        <v>61</v>
+      </c>
+      <c r="L41">
+        <v>4</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>78</v>
+      </c>
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" t="s">
+        <v>79</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43" t="s">
+        <v>90</v>
+      </c>
+      <c r="J43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K43" t="s">
+        <v>61</v>
+      </c>
+      <c r="L43">
+        <v>7</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44" t="s">
+        <v>93</v>
+      </c>
+      <c r="J44" t="s">
+        <v>49</v>
+      </c>
+      <c r="K44" t="s">
+        <v>88</v>
+      </c>
+      <c r="L44">
+        <v>3</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <v>6</v>
+      </c>
+      <c r="I45" t="s">
+        <v>76</v>
+      </c>
+      <c r="J45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K45" t="s">
+        <v>65</v>
+      </c>
+      <c r="L45">
+        <v>12</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46" t="s">
+        <v>74</v>
+      </c>
+      <c r="J46" t="s">
+        <v>49</v>
+      </c>
+      <c r="K46" t="s">
+        <v>14</v>
+      </c>
+      <c r="L46">
+        <v>3</v>
+      </c>
+      <c r="S46" s="2"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>193</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" t="s">
+        <v>20</v>
+      </c>
+      <c r="L47">
+        <v>6</v>
+      </c>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="X47" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K32" xr:uid="{6CB10BF2-3928-447D-99A5-1738F96EC912}">
+  <autoFilter ref="C1:L32" xr:uid="{6CB10BF2-3928-447D-99A5-1738F96EC912}">
     <filterColumn colId="2" showButton="0"/>
   </autoFilter>
   <mergeCells count="2">
-    <mergeCell ref="L1:Y1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="M1:Z1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2053,10 +2750,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EACDF8E-1BC9-48C7-AB83-F83733DC582C}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AO16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,30 +2790,35 @@
     <col min="29" max="29" width="14.5546875" customWidth="1"/>
     <col min="30" max="30" width="10" customWidth="1"/>
     <col min="31" max="31" width="5.21875" customWidth="1"/>
-    <col min="32" max="32" width="6.6640625" customWidth="1"/>
+    <col min="32" max="32" width="5.6640625" customWidth="1"/>
+    <col min="33" max="33" width="6.21875" customWidth="1"/>
+    <col min="34" max="34" width="6.6640625" customWidth="1"/>
+    <col min="35" max="35" width="6.33203125" customWidth="1"/>
+    <col min="36" max="36" width="7.33203125" customWidth="1"/>
+    <col min="37" max="37" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="3" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" s="3" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -2140,7 +2843,7 @@
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
     </row>
-    <row r="2" spans="1:34" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -2159,7 +2862,7 @@
         <v>33</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>34</v>
@@ -2183,65 +2886,86 @@
         <v>40</v>
       </c>
       <c r="V2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="X2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AC2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AD2" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="AE2" s="3" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I3" s="7">
         <v>40</v>
@@ -2270,12 +2994,12 @@
       <c r="AE3" s="9"/>
       <c r="AF3" s="9"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -2310,24 +3034,24 @@
       <c r="AE4" s="7"/>
       <c r="AF4" s="7"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" s="7">
         <v>40</v>
@@ -2356,21 +3080,21 @@
       <c r="AE5" s="9"/>
       <c r="AF5" s="9"/>
     </row>
-    <row r="6" spans="1:34" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>28</v>
@@ -2384,21 +3108,21 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>28</v>
@@ -2412,21 +3136,21 @@
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" s="7">
         <v>15</v>
@@ -2436,15 +3160,15 @@
       <c r="V8" s="2"/>
       <c r="AG8" s="2"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I9" s="7">
         <v>7</v>
@@ -2456,12 +3180,12 @@
       <c r="V9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I10" s="7">
         <v>2</v>
@@ -2470,15 +3194,15 @@
       <c r="P10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:34" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I11" s="7">
         <v>15</v>
@@ -2490,15 +3214,15 @@
       <c r="V11" s="2"/>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" s="7">
         <v>3</v>
@@ -2509,6 +3233,94 @@
       <c r="Q12" s="2"/>
       <c r="V12" s="2"/>
       <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="7">
+        <v>50</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AI13" s="2"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="7">
+        <v>20</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AI14" s="2"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I15" s="7">
+        <v>2</v>
+      </c>
+      <c r="V15" s="2"/>
+      <c r="AJ15" s="2"/>
+    </row>
+    <row r="16" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" s="7">
+        <v>2</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
IceWindDale - added potions; Castle clash - heroes added
</commit_message>
<xml_diff>
--- a/IceWind_Dale/equipment.xlsx
+++ b/IceWind_Dale/equipment.xlsx
@@ -9,16 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Broń" sheetId="1" r:id="rId1"/>
     <sheet name="Zbroja" sheetId="2" r:id="rId2"/>
+    <sheet name="Mikstury" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Broń!$C$1:$L$32</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="262">
   <si>
     <t>Nazwa broni</t>
   </si>
@@ -682,6 +684,138 @@
   </si>
   <si>
     <t>Miecz Baela +3</t>
+  </si>
+  <si>
+    <t>Nazwa</t>
+  </si>
+  <si>
+    <t>Mikstura uzdrowienia</t>
+  </si>
+  <si>
+    <t>Eliksir zdrowia</t>
+  </si>
+  <si>
+    <t>Neutralizuje trucizny i choroby oraz przywraca 10 punktów życia</t>
+  </si>
+  <si>
+    <t>Antidotum</t>
+  </si>
+  <si>
+    <t>Neutralizuje truciznę</t>
+  </si>
+  <si>
+    <t>Mikstura odporności na ogień</t>
+  </si>
+  <si>
+    <t>Mikstura siły lodowego olbrzyma</t>
+  </si>
+  <si>
+    <t>Mikstura niewrażliwości</t>
+  </si>
+  <si>
+    <t>Olej wściekłego płomienia</t>
+  </si>
+  <si>
+    <t>Obrażenia: 5k6 od ognia (połowa po rzucie obronnym przeciw zionięciom), zasięg: 13 metrów, obszar działania: w promieniu 10 metrów</t>
+  </si>
+  <si>
+    <t>Dwukrotnie zwiększa prędkość poruszania się i ataku</t>
+  </si>
+  <si>
+    <t>Czas działania</t>
+  </si>
+  <si>
+    <t>Natychmiastowy</t>
+  </si>
+  <si>
+    <t>Przywraca 9 punktów życia</t>
+  </si>
+  <si>
+    <t>2 godziny</t>
+  </si>
+  <si>
+    <t>1 godzina</t>
+  </si>
+  <si>
+    <t>Odporność na ogień: +50%</t>
+  </si>
+  <si>
+    <t>Siła: 21 (siła lodowego olbrzyma)</t>
+  </si>
+  <si>
+    <t>Klasa pancerza: 0, Rzuty obronne: +5</t>
+  </si>
+  <si>
+    <t>Mikstura zręczności</t>
+  </si>
+  <si>
+    <t>Zręczność: 18</t>
+  </si>
+  <si>
+    <t>15 tur</t>
+  </si>
+  <si>
+    <t>Olej szybkości</t>
+  </si>
+  <si>
+    <t>Mikstura infrawizji</t>
+  </si>
+  <si>
+    <t>Infrawizja</t>
+  </si>
+  <si>
+    <t>4 godziny</t>
+  </si>
+  <si>
+    <t>Mikstura skupienia</t>
+  </si>
+  <si>
+    <t>Inteligencja: +3, Zręczność: +3</t>
+  </si>
+  <si>
+    <t>12 godzin</t>
+  </si>
+  <si>
+    <t>Mikstura lustrzanych oczu</t>
+  </si>
+  <si>
+    <t>Niewrażliwość na petryfikację</t>
+  </si>
+  <si>
+    <t>1 tura</t>
+  </si>
+  <si>
+    <t>Mikstura wolności</t>
+  </si>
+  <si>
+    <t>Swoboda działania</t>
+  </si>
+  <si>
+    <t>Napar mumii</t>
+  </si>
+  <si>
+    <t>Leczy ślepotę, głuchotę i choroby</t>
+  </si>
+  <si>
+    <t>Płonąca oliwa</t>
+  </si>
+  <si>
+    <t>Po trafieniu w cel, szklane naczynie rozbija się, rozlewając płonącą oliwę na wszystko w promieniu 1,5 metra, powodując 2k8 obrażeń od ognia</t>
+  </si>
+  <si>
+    <t>Mikstura heroizmu</t>
+  </si>
+  <si>
+    <t>Punkty życia: +10% (tylko bazowe), TraK0: 90% bazowej wartości</t>
+  </si>
+  <si>
+    <t>Mikstura niewidzialności</t>
+  </si>
+  <si>
+    <t>Niewidzialność</t>
+  </si>
+  <si>
+    <t>24 godziny</t>
   </si>
 </sst>
 </file>
@@ -706,7 +840,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,8 +859,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -734,38 +874,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1083,2064 +1293,2086 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="26.88671875" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" customWidth="1"/>
-    <col min="13" max="13" width="4.88671875" customWidth="1"/>
-    <col min="14" max="14" width="5.109375" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" customWidth="1"/>
-    <col min="16" max="16" width="8.21875" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" customWidth="1"/>
-    <col min="18" max="18" width="9.88671875" customWidth="1"/>
-    <col min="19" max="19" width="4.88671875" customWidth="1"/>
-    <col min="20" max="20" width="4.77734375" customWidth="1"/>
-    <col min="21" max="21" width="9.44140625" customWidth="1"/>
-    <col min="22" max="22" width="9.5546875" customWidth="1"/>
-    <col min="23" max="23" width="14.77734375" customWidth="1"/>
-    <col min="24" max="24" width="5.44140625" customWidth="1"/>
-    <col min="25" max="25" width="5.5546875" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" customWidth="1"/>
-    <col min="27" max="27" width="6.21875" customWidth="1"/>
-    <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.109375" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
-    <col min="31" max="31" width="10.44140625" customWidth="1"/>
-    <col min="32" max="32" width="14.5546875" customWidth="1"/>
-    <col min="33" max="33" width="10" customWidth="1"/>
-    <col min="34" max="34" width="18.6640625" customWidth="1"/>
-    <col min="35" max="35" width="16.109375" customWidth="1"/>
-    <col min="36" max="36" width="18.33203125" customWidth="1"/>
-    <col min="37" max="37" width="15.33203125" customWidth="1"/>
-    <col min="38" max="38" width="14.21875" customWidth="1"/>
-    <col min="39" max="39" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="4"/>
+    <col min="11" max="11" width="11.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="4.88671875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="5.109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="5.88671875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="8.21875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" style="4" customWidth="1"/>
+    <col min="19" max="19" width="4.88671875" style="4" customWidth="1"/>
+    <col min="20" max="20" width="4.77734375" style="4" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="9.5546875" style="4" customWidth="1"/>
+    <col min="23" max="23" width="14.77734375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="5.44140625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="5.5546875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" style="4" customWidth="1"/>
+    <col min="27" max="27" width="6.21875" style="4" customWidth="1"/>
+    <col min="28" max="28" width="6" style="4" customWidth="1"/>
+    <col min="29" max="29" width="5.109375" style="4" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" style="4" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" style="4" customWidth="1"/>
+    <col min="32" max="32" width="14.5546875" style="4" customWidth="1"/>
+    <col min="33" max="33" width="10" style="4" customWidth="1"/>
+    <col min="34" max="34" width="18.6640625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="16.109375" style="4" customWidth="1"/>
+    <col min="36" max="36" width="18.33203125" style="4" customWidth="1"/>
+    <col min="37" max="37" width="15.33203125" style="4" customWidth="1"/>
+    <col min="38" max="38" width="14.21875" style="4" customWidth="1"/>
+    <col min="39" max="39" width="16.5546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:39" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-    </row>
-    <row r="2" spans="1:39" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3" t="s">
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+    </row>
+    <row r="2" spans="1:39" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL2" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="6" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>3</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>6</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="X4" s="5"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>7</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="4">
         <v>7</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="4">
         <v>4</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="X6" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="4">
         <v>3</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="4">
         <v>8</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="X8" s="2"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="X8" s="5"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>8</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="4">
         <v>5</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
+      <c r="M9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>7</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="4">
         <v>12</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="X10" s="2"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="X10" s="5"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <v>8</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="4">
         <v>10</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <v>10</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="4">
         <v>15</v>
       </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>5</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="4">
         <v>4</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
+      <c r="M13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="4">
         <v>4</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="4">
         <v>6</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>7</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="4">
         <v>15</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="X15" s="2"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="X15" s="5"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>4</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="4">
         <v>4</v>
       </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4">
         <v>4</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="4">
         <v>4</v>
       </c>
-      <c r="S17" s="2"/>
+      <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="4">
         <v>9</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="4">
         <v>15</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="4">
         <v>2</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="4">
         <v>1</v>
       </c>
-      <c r="M19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
+      <c r="M19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="4">
         <v>2</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="4">
         <v>0</v>
       </c>
-      <c r="M20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
+      <c r="M20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="4">
         <v>2</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="4">
         <v>0</v>
       </c>
-      <c r="M21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
+      <c r="M21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="4">
         <v>10</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="4">
         <v>14</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="4">
         <v>5</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="4">
         <v>7</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="Y23" s="2"/>
-      <c r="Z23" s="2"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="4">
         <v>7</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="4">
         <v>3</v>
       </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="2"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="4">
         <v>7</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="4">
         <v>10</v>
       </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="4">
         <v>6</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="4">
         <v>2</v>
       </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="2"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="4">
         <v>6</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="4">
         <v>0</v>
       </c>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="2"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="4">
         <v>0</v>
       </c>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="AA28" s="2"/>
-      <c r="AB28" s="2"/>
-      <c r="AC28" s="2"/>
-      <c r="AD28" s="2"/>
-      <c r="AE28" s="2"/>
-      <c r="AF28" s="2"/>
-      <c r="AG28" s="2"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="4">
         <v>0</v>
       </c>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="2"/>
-      <c r="AD29" s="2"/>
-      <c r="AE29" s="2"/>
-      <c r="AF29" s="2"/>
-      <c r="AG29" s="2"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="AA29" s="14"/>
+      <c r="AB29" s="14"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="4">
         <v>1</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="4">
         <v>1</v>
       </c>
-      <c r="M31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
+      <c r="M31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="4">
         <v>2</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="4">
         <v>1</v>
       </c>
-      <c r="M32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
-      <c r="X32" s="2"/>
+      <c r="M32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="4">
         <v>5</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="4">
         <v>2</v>
       </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="4">
         <v>7</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="4">
         <v>9</v>
       </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="4">
         <v>2</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="4">
         <v>3</v>
       </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
     </row>
     <row r="36" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="4">
         <v>5</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="4">
         <v>5</v>
       </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
     </row>
     <row r="37" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="4">
         <v>5</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="4">
         <v>0</v>
       </c>
-      <c r="Y37" s="2"/>
-      <c r="Z37" s="2"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
     </row>
     <row r="38" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="4">
         <v>5</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="4">
         <v>2</v>
       </c>
-      <c r="M38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
-      <c r="X38" s="2"/>
+      <c r="M38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
     </row>
     <row r="39" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="4">
         <v>1</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="4">
         <v>3</v>
       </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="5"/>
+      <c r="X39" s="5"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="4">
         <v>3</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="4">
         <v>5</v>
       </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="X40" s="2"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="X40" s="5"/>
     </row>
     <row r="41" spans="1:26" ht="72" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="4">
         <v>4</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="4">
         <v>4</v>
       </c>
-      <c r="M41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="R41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
-      <c r="X41" s="2"/>
+      <c r="M41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="4">
         <v>1</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="4">
         <v>1</v>
       </c>
-      <c r="M42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
-      <c r="X42" s="2"/>
+      <c r="M42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="4">
         <v>4</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="4">
         <v>7</v>
       </c>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
-      <c r="Y43" s="2"/>
-      <c r="Z43" s="2"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="4">
         <v>4</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="4">
         <v>3</v>
       </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
-      <c r="Y44" s="2"/>
-      <c r="Z44" s="2"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="4">
         <v>6</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K45" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="4">
         <v>12</v>
       </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="4">
         <v>1</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="4">
         <v>3</v>
       </c>
-      <c r="S46" s="2"/>
+      <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="4">
         <v>1</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="4">
         <v>6</v>
       </c>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="X47" s="2"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="X47" s="5"/>
     </row>
     <row r="48" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="4">
         <v>3</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K48" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="4">
         <v>2</v>
       </c>
-      <c r="O48" s="1"/>
+      <c r="O48" s="14"/>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="4">
         <v>7</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K49" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="4">
         <v>8</v>
       </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-      <c r="X49" s="2"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
     </row>
     <row r="50" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="4">
         <v>5</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K50" t="s">
+      <c r="K50" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="4">
         <v>7</v>
       </c>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
-      <c r="X50" s="2"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="X50" s="5"/>
     </row>
     <row r="51" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="4">
         <v>6</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="4">
         <v>8</v>
       </c>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="R51" s="2"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="2"/>
-      <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
-      <c r="X51" s="2"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
     </row>
     <row r="52" spans="1:39" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="4">
         <v>4</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K52" t="s">
+      <c r="K52" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="4">
         <v>9</v>
       </c>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="2"/>
-      <c r="U52" s="2"/>
-      <c r="X52" s="2"/>
-      <c r="AH52" s="2"/>
-      <c r="AI52" s="2"/>
-      <c r="AJ52" s="2"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="X52" s="5"/>
+      <c r="AH52" s="5"/>
+      <c r="AI52" s="5"/>
+      <c r="AJ52" s="5"/>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="4">
         <v>6</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K53" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="4">
         <v>10</v>
       </c>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="R53" s="2"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="2"/>
-      <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
-      <c r="W53" s="2"/>
-      <c r="X53" s="2"/>
-      <c r="AK53" s="2"/>
-      <c r="AL53" s="2"/>
-      <c r="AM53" s="2"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="AK53" s="5"/>
+      <c r="AL53" s="5"/>
+      <c r="AM53" s="5"/>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="4">
         <v>4</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K54" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L54">
+      <c r="L54" s="4">
         <v>4</v>
       </c>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-      <c r="R54" s="2"/>
-      <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
-      <c r="W54" s="2"/>
-      <c r="X54" s="2"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="4">
         <v>3</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K55" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L55">
+      <c r="L55" s="4">
         <v>4</v>
       </c>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
-      <c r="R55" s="2"/>
-      <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
-      <c r="X55" s="2"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:L32" xr:uid="{6CB10BF2-3928-447D-99A5-1738F96EC912}">
@@ -3160,574 +3392,597 @@
   <dimension ref="A1:AO16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.88671875" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" customWidth="1"/>
-    <col min="13" max="13" width="8.21875" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" customWidth="1"/>
-    <col min="17" max="17" width="4.77734375" customWidth="1"/>
-    <col min="18" max="18" width="9.44140625" customWidth="1"/>
-    <col min="19" max="19" width="9.5546875" customWidth="1"/>
-    <col min="20" max="20" width="14.77734375" customWidth="1"/>
-    <col min="21" max="21" width="5.44140625" customWidth="1"/>
-    <col min="22" max="22" width="5.5546875" customWidth="1"/>
-    <col min="23" max="23" width="6.109375" customWidth="1"/>
-    <col min="24" max="24" width="6.21875" customWidth="1"/>
-    <col min="25" max="25" width="6" customWidth="1"/>
-    <col min="26" max="26" width="5.109375" customWidth="1"/>
-    <col min="27" max="27" width="5.44140625" customWidth="1"/>
-    <col min="28" max="28" width="10.44140625" customWidth="1"/>
-    <col min="29" max="29" width="14.5546875" customWidth="1"/>
-    <col min="30" max="30" width="10" customWidth="1"/>
-    <col min="31" max="31" width="5.21875" customWidth="1"/>
-    <col min="32" max="32" width="5.6640625" customWidth="1"/>
-    <col min="33" max="33" width="6.21875" customWidth="1"/>
-    <col min="34" max="34" width="6.6640625" customWidth="1"/>
-    <col min="35" max="35" width="6.33203125" customWidth="1"/>
-    <col min="36" max="36" width="7.33203125" customWidth="1"/>
-    <col min="37" max="37" width="10" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" style="13" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="5.109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.21875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="4.88671875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="4.77734375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="9.44140625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" style="4" customWidth="1"/>
+    <col min="20" max="20" width="14.77734375" style="4" customWidth="1"/>
+    <col min="21" max="21" width="5.44140625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="5.5546875" style="4" customWidth="1"/>
+    <col min="23" max="23" width="6.109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="6.21875" style="4" customWidth="1"/>
+    <col min="25" max="25" width="6" style="4" customWidth="1"/>
+    <col min="26" max="26" width="5.109375" style="4" customWidth="1"/>
+    <col min="27" max="27" width="5.44140625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="10.44140625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="14.5546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="10" style="4" customWidth="1"/>
+    <col min="31" max="31" width="5.21875" style="4" customWidth="1"/>
+    <col min="32" max="32" width="5.6640625" style="4" customWidth="1"/>
+    <col min="33" max="33" width="6.21875" style="4" customWidth="1"/>
+    <col min="34" max="34" width="6.6640625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="6.33203125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="7.33203125" style="4" customWidth="1"/>
+    <col min="37" max="37" width="10" style="4" customWidth="1"/>
+    <col min="38" max="41" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:41" s="1" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-    </row>
-    <row r="2" spans="1:41" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+    </row>
+    <row r="2" spans="1:41" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AN2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AO2" s="6" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="9">
         <v>40</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
         <v>2</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="9">
         <v>40</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
     </row>
     <row r="6" spans="1:41" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="9">
         <v>40</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
+      <c r="L6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
     </row>
     <row r="7" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="9">
         <v>25</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
+      <c r="L7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="9">
         <v>15</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="AG8" s="2"/>
+      <c r="L8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="AG8" s="5"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="9">
         <v>7</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="X9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="9">
         <v>2</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="V10" s="2"/>
+      <c r="L10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:41" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="9">
         <v>15</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="X11" s="2"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="9">
         <v>3</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="X12" s="1"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="X12" s="14"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="9">
         <v>50</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AI13" s="2"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AI13" s="5"/>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="9">
         <v>20</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AI14" s="2"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AI14" s="5"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="9">
         <v>2</v>
       </c>
-      <c r="V15" s="2"/>
-      <c r="AJ15" s="2"/>
+      <c r="V15" s="5"/>
+      <c r="AJ15" s="5"/>
     </row>
     <row r="16" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="9">
         <v>2</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="AK16" s="2"/>
-      <c r="AL16" s="2"/>
-      <c r="AM16" s="2"/>
-      <c r="AN16" s="2"/>
-      <c r="AO16" s="2"/>
+      <c r="L16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3736,4 +3991,346 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FF04B9-A048-4F7D-8D58-D478FFC7F680}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="70" style="9" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="5.21875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IceWindDale - new equipment added
</commit_message>
<xml_diff>
--- a/IceWind_Dale/equipment.xlsx
+++ b/IceWind_Dale/equipment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Broń" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="268">
   <si>
     <t>Nazwa broni</t>
   </si>
@@ -452,27 +452,15 @@
     <t>Tarcza średnia</t>
   </si>
   <si>
-    <t>Klasa pancerza: +1</t>
-  </si>
-  <si>
     <t>Puklerz</t>
   </si>
   <si>
-    <t>Klasa pancerza: +1, nie chroni przed obrażeniami kłutymi i pociskami</t>
-  </si>
-  <si>
     <t>Pawęż</t>
   </si>
   <si>
-    <t>Klasa pancerza: +1, (+2 przeciw pociskom)</t>
-  </si>
-  <si>
     <t>Mała tarcza</t>
   </si>
   <si>
-    <t>Klasa pancerza: +1, nie chroni przed pociskami</t>
-  </si>
-  <si>
     <t>Zbroja płytowa</t>
   </si>
   <si>
@@ -512,9 +500,6 @@
     <t>Chełm zaufanego obrońcy</t>
   </si>
   <si>
-    <t>klasa pancerza: +3, niewrażliwość na uśpienie i zmęczenie, chroni przed obrażeniami krytycznymi</t>
-  </si>
-  <si>
     <t>Krasnolud</t>
   </si>
   <si>
@@ -816,6 +801,39 @@
   </si>
   <si>
     <t>24 godziny</t>
+  </si>
+  <si>
+    <t>Nie chroni przed obrażeniami kłutymi i pociskami</t>
+  </si>
+  <si>
+    <t>Niewrażliwość na uśpienie i zmęczenie, chroni przed obrażeniami krytycznymi</t>
+  </si>
+  <si>
+    <t>Wekiera wysokiej jakości</t>
+  </si>
+  <si>
+    <t>Pas beatyfikacji</t>
+  </si>
+  <si>
+    <t>Użytkownik znajduje się pod wpływem czaru Błogosławieństwo</t>
+  </si>
+  <si>
+    <t>Różdźka szukania pułapek</t>
+  </si>
+  <si>
+    <t>Właściwości ładunków - znajdowanie pułapek; Użytkownik wykrywa pułapki jakby był złodziejem</t>
+  </si>
+  <si>
+    <t>inteligencja:9</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Zbroja skórzana +1</t>
+  </si>
+  <si>
+    <t>Miecz długi najlepszej jakości</t>
   </si>
 </sst>
 </file>
@@ -866,7 +884,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -926,11 +944,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -941,12 +985,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -965,6 +1003,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -974,8 +1042,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1291,19 +1368,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM55"/>
+  <dimension ref="A1:AM57"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="25" style="7" customWidth="1"/>
     <col min="2" max="2" width="29.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="11" customWidth="1"/>
     <col min="5" max="5" width="16.109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="15.88671875" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.88671875" style="4" customWidth="1"/>
@@ -1342,87 +1419,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="16"/>
     </row>
     <row r="2" spans="1:39" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="6" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
       <c r="M2" s="6" t="s">
         <v>30</v>
       </c>
@@ -1487,29 +1564,29 @@
         <v>107</v>
       </c>
       <c r="AH2" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AJ2" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AL2" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="AK2" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AL2" s="6" t="s">
-        <v>214</v>
-      </c>
       <c r="AM2" s="6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1530,7 +1607,7 @@
       <c r="L3" s="4">
         <v>3</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="12" t="s">
         <v>29</v>
       </c>
       <c r="N3" s="5"/>
@@ -1543,10 +1620,10 @@
       <c r="X3" s="5"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1575,10 +1652,10 @@
       <c r="X4" s="5"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1599,13 +1676,13 @@
       <c r="L5" s="4">
         <v>7</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="12" t="s">
         <v>29</v>
       </c>
       <c r="R5" s="5"/>
@@ -1617,10 +1694,10 @@
       <c r="X5" s="5"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1641,39 +1718,39 @@
       <c r="L6" s="4">
         <v>4</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="V6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="W6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="X6" s="14" t="s">
+      <c r="X6" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1697,10 +1774,10 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1729,10 +1806,10 @@
       <c r="X8" s="5"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1763,10 +1840,10 @@
       <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1795,10 +1872,10 @@
       <c r="X10" s="5"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -1831,10 +1908,10 @@
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="A12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1867,10 +1944,10 @@
       <c r="X12" s="5"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1900,10 +1977,10 @@
       <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1935,10 +2012,10 @@
       <c r="X14" s="5"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1967,10 +2044,10 @@
       <c r="X15" s="5"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -2008,10 +2085,10 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -2035,10 +2112,10 @@
       <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -2071,10 +2148,10 @@
       <c r="X18" s="5"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -2104,10 +2181,10 @@
       <c r="X19" s="5"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -2139,10 +2216,10 @@
       <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>83</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -2170,13 +2247,13 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="11" t="s">
         <v>86</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -2210,10 +2287,10 @@
       <c r="Z22" s="5"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="11" t="s">
         <v>86</v>
       </c>
       <c r="H23" s="4">
@@ -2244,10 +2321,10 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>92</v>
       </c>
       <c r="H24" s="4">
@@ -2278,13 +2355,13 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="11" t="s">
         <v>92</v>
       </c>
       <c r="H25" s="4">
@@ -2315,7 +2392,7 @@
       <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H26" s="4">
@@ -2345,7 +2422,7 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H27" s="4">
@@ -2367,10 +2444,10 @@
       <c r="Z27" s="5"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -2393,10 +2470,10 @@
       <c r="AG28" s="5"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -2410,8 +2487,8 @@
       </c>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
-      <c r="AA29" s="14"/>
-      <c r="AB29" s="14"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
       <c r="AE29" s="5"/>
@@ -2419,10 +2496,10 @@
       <c r="AG29" s="5"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="4" t="s">
@@ -2436,13 +2513,13 @@
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="11" t="s">
         <v>92</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -2472,13 +2549,13 @@
       <c r="X31" s="5"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="11" t="s">
         <v>92</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -2508,13 +2585,13 @@
       <c r="X32" s="5"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="13" t="s">
+      <c r="A33" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="11" t="s">
         <v>92</v>
       </c>
       <c r="H33" s="4">
@@ -2545,13 +2622,13 @@
       <c r="Z33" s="5"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D34" s="13" t="s">
+      <c r="A34" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>92</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -2584,13 +2661,13 @@
       <c r="X34" s="5"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" s="13" t="s">
+      <c r="A35" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="11" t="s">
         <v>92</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -2622,16 +2699,16 @@
       <c r="X35" s="5"/>
     </row>
     <row r="36" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D36" s="13" t="s">
+      <c r="A36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>86</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -2664,14 +2741,14 @@
       <c r="X36" s="5"/>
     </row>
     <row r="37" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>171</v>
+      <c r="A37" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="H37" s="4">
         <v>5</v>
@@ -2692,17 +2769,17 @@
       <c r="Z37" s="5"/>
     </row>
     <row r="38" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C38" s="13" t="s">
+      <c r="A38" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>174</v>
+      <c r="B38" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>11</v>
@@ -2732,19 +2809,19 @@
       <c r="X38" s="5"/>
     </row>
     <row r="39" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E39" s="9" t="s">
+      <c r="A39" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="4">
@@ -2773,14 +2850,14 @@
       <c r="X39" s="5"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D40" s="13" t="s">
+      <c r="A40" s="7" t="s">
         <v>174</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>18</v>
@@ -2808,16 +2885,16 @@
       <c r="X40" s="5"/>
     </row>
     <row r="41" spans="1:26" ht="72" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D41" s="13" t="s">
+      <c r="A41" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>86</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -2847,14 +2924,14 @@
       <c r="X41" s="5"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>185</v>
+      <c r="A42" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>11</v>
@@ -2883,14 +2960,14 @@
       <c r="X42" s="5"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>187</v>
+      <c r="A43" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>69</v>
@@ -2923,14 +3000,14 @@
       <c r="Z43" s="5"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>185</v>
+      <c r="A44" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="H44" s="4">
         <v>4</v>
@@ -2960,14 +3037,14 @@
       <c r="Z44" s="5"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>174</v>
+      <c r="A45" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>11</v>
@@ -2999,14 +3076,14 @@
       <c r="X45" s="5"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>174</v>
+      <c r="A46" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>18</v>
@@ -3029,14 +3106,14 @@
       <c r="S46" s="5"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>174</v>
+      <c r="A47" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>18</v>
@@ -3064,16 +3141,16 @@
       <c r="X47" s="5"/>
     </row>
     <row r="48" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E48" s="9" t="s">
+      <c r="A48" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>18</v>
       </c>
       <c r="H48" s="4">
@@ -3091,17 +3168,17 @@
       <c r="L48" s="4">
         <v>2</v>
       </c>
-      <c r="O48" s="14"/>
+      <c r="O48" s="12"/>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>174</v>
+      <c r="A49" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>23</v>
@@ -3133,17 +3210,17 @@
       <c r="X49" s="5"/>
     </row>
     <row r="50" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>174</v>
+      <c r="A50" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>18</v>
@@ -3171,17 +3248,17 @@
       <c r="X50" s="5"/>
     </row>
     <row r="51" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>203</v>
+      <c r="A51" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="H51" s="4">
         <v>6</v>
@@ -3210,17 +3287,17 @@
       <c r="X51" s="5"/>
     </row>
     <row r="52" spans="1:39" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>174</v>
+      <c r="A52" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>18</v>
@@ -3251,17 +3328,17 @@
       <c r="AJ52" s="5"/>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>210</v>
+      <c r="A53" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>174</v>
+        <v>206</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>23</v>
@@ -3296,17 +3373,17 @@
       <c r="AM53" s="5"/>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>174</v>
+      <c r="A54" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>23</v>
@@ -3337,14 +3414,14 @@
       <c r="X54" s="5"/>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>174</v>
+      <c r="A55" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>23</v>
@@ -3374,13 +3451,95 @@
       <c r="W55" s="5"/>
       <c r="X55" s="5"/>
     </row>
+    <row r="56" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" s="4">
+        <v>7</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L56" s="4">
+        <v>8</v>
+      </c>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="X56" s="5"/>
+    </row>
+    <row r="57" spans="1:39" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H57" s="4">
+        <v>5</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L57" s="4">
+        <v>4</v>
+      </c>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+    </row>
   </sheetData>
   <autoFilter ref="C1:L32" xr:uid="{6CB10BF2-3928-447D-99A5-1738F96EC912}">
     <filterColumn colId="2" showButton="0"/>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="M1:Z1"/>
+  <mergeCells count="11">
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="M1:AM1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3389,23 +3548,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EACDF8E-1BC9-48C7-AB83-F83733DC582C}">
-  <dimension ref="A1:AO16"/>
+  <dimension ref="A1:AP19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="35.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="4" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" style="4" customWidth="1"/>
     <col min="10" max="10" width="4.88671875" style="4" customWidth="1"/>
     <col min="11" max="11" width="5.109375" style="4" customWidth="1"/>
@@ -3433,84 +3592,85 @@
     <col min="33" max="33" width="6.21875" style="4" customWidth="1"/>
     <col min="34" max="34" width="6.6640625" style="4" customWidth="1"/>
     <col min="35" max="35" width="6.33203125" style="4" customWidth="1"/>
-    <col min="36" max="36" width="7.33203125" style="4" customWidth="1"/>
-    <col min="37" max="37" width="10" style="4" customWidth="1"/>
-    <col min="38" max="41" width="8.88671875" style="4"/>
+    <col min="36" max="37" width="7.33203125" style="4" customWidth="1"/>
+    <col min="38" max="38" width="10" style="4" customWidth="1"/>
+    <col min="39" max="42" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:42" s="1" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-    </row>
-    <row r="2" spans="1:41" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="23"/>
+    </row>
+    <row r="2" spans="1:42" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="6" t="s">
         <v>30</v>
       </c>
@@ -3575,7 +3735,7 @@
         <v>107</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AF2" s="6" t="s">
         <v>122</v>
@@ -3590,178 +3750,181 @@
         <v>102</v>
       </c>
       <c r="AJ2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN2" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AK2" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="AL2" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="AM2" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="AN2" s="6" t="s">
-        <v>164</v>
-      </c>
       <c r="AO2" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="7">
         <v>40</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="J3" s="7"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7">
         <v>2</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>40</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-    </row>
-    <row r="6" spans="1:41" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="J5" s="7"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+    </row>
+    <row r="6" spans="1:42" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>40</v>
       </c>
       <c r="L6" s="5"/>
@@ -3770,26 +3933,26 @@
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
     </row>
-    <row r="7" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="7">
         <v>25</v>
       </c>
       <c r="L7" s="5"/>
@@ -3798,23 +3961,23 @@
       <c r="AG7" s="5"/>
       <c r="AH7" s="5"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="7">
         <v>15</v>
       </c>
       <c r="L8" s="5"/>
@@ -3822,17 +3985,17 @@
       <c r="V8" s="5"/>
       <c r="AG8" s="5"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="C9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>7</v>
       </c>
       <c r="K9" s="5"/>
@@ -3842,31 +4005,38 @@
       <c r="V9" s="5"/>
       <c r="X9" s="5"/>
     </row>
-    <row r="10" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="I10" s="9">
+    <row r="10" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="7">
         <v>2</v>
       </c>
       <c r="L10" s="5"/>
       <c r="P10" s="5"/>
       <c r="V10" s="5"/>
     </row>
-    <row r="11" spans="1:41" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="9" t="s">
+    <row r="11" spans="1:42" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>15</v>
       </c>
       <c r="K11" s="5"/>
@@ -3876,17 +4046,18 @@
       <c r="V11" s="5"/>
       <c r="X11" s="5"/>
     </row>
-    <row r="12" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H12" s="9" t="s">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>3</v>
       </c>
       <c r="K12" s="5"/>
@@ -3894,22 +4065,22 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="V12" s="5"/>
-      <c r="X12" s="14"/>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="X12" s="12"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="D13" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="7">
         <v>50</v>
       </c>
       <c r="K13" s="5"/>
@@ -3923,20 +4094,20 @@
       <c r="AF13" s="5"/>
       <c r="AI13" s="5"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="13" t="s">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="D14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="7">
         <v>20</v>
       </c>
       <c r="K14" s="5"/>
@@ -3950,27 +4121,30 @@
       <c r="AF14" s="5"/>
       <c r="AI14" s="5"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="13" t="s">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <v>2</v>
       </c>
       <c r="V15" s="5"/>
       <c r="AJ15" s="5"/>
     </row>
-    <row r="16" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="I16" s="9">
+    <row r="16" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="I16" s="7">
         <v>2</v>
       </c>
       <c r="L16" s="5"/>
@@ -3978,15 +4152,81 @@
       <c r="Q16" s="5"/>
       <c r="V16" s="5"/>
       <c r="X16" s="5"/>
-      <c r="AK16" s="5"/>
       <c r="AL16" s="5"/>
       <c r="AM16" s="5"/>
       <c r="AN16" s="5"/>
       <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+    </row>
+    <row r="17" spans="1:37" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="AJ17" s="5"/>
+    </row>
+    <row r="18" spans="1:37" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="4">
+        <v>10</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="AK19" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="J1:W1"/>
+  <mergeCells count="10">
+    <mergeCell ref="J1:AP1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3997,16 +4237,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FF04B9-A048-4F7D-8D58-D478FFC7F680}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="70" style="9" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="70" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" style="7" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="4"/>
     <col min="5" max="5" width="5.21875" style="4" customWidth="1"/>
     <col min="6" max="6" width="5" style="4" customWidth="1"/>
@@ -4017,34 +4257,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="16" t="s">
+      <c r="A1" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>102</v>
@@ -4063,56 +4303,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>231</v>
+      <c r="A3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>231</v>
+      <c r="A4" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>231</v>
+      <c r="A5" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>233</v>
+      <c r="A6" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -4120,14 +4360,14 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>233</v>
+      <c r="A7" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -4140,14 +4380,14 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>234</v>
+      <c r="A8" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -4160,14 +4400,14 @@
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>231</v>
+      <c r="A9" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -4175,14 +4415,14 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -4190,14 +4430,14 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>240</v>
+      <c r="A11" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4205,14 +4445,14 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>244</v>
+      <c r="A12" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -4220,14 +4460,14 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>247</v>
+      <c r="A13" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -4235,14 +4475,14 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>250</v>
+      <c r="A14" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -4250,14 +4490,14 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>233</v>
+      <c r="A15" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -4265,42 +4505,42 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>231</v>
+      <c r="A16" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>231</v>
+      <c r="A17" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="D17" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>233</v>
+      <c r="A18" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -4313,14 +4553,14 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>261</v>
+      <c r="A19" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -4328,8 +4568,12 @@
       <c r="E19" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>